<commit_message>
Deploying to gh-pages from  @ 3f0716d2d48660f8e0c43ea006289a326d9f4010 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2021_5-1-1.xlsx
+++ b/assets/excel/2021_5-1-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\GitHub\IM_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D378E8-C42C-4463-9EF1-F74E547B81A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{72E96349-9798-4592-BDED-9F3BD5F94922}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13110" xr2:uid="{F2F2BFBB-2123-4078-9F45-2FAEA1EAACE2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" xr2:uid="{F2F2BFBB-2123-4078-9F45-2FAEA1EAACE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="31">
   <si>
     <t>Migration und Teilhabe in Niedersachsen - Integrationsmonitoring 2021</t>
   </si>
@@ -124,30 +124,6 @@
     <t>/</t>
   </si>
   <si>
-    <t>Land- und Forstwirtschaft; Fischerei und Fischzucht</t>
-  </si>
-  <si>
-    <t>Energie- und Wasserversorgung</t>
-  </si>
-  <si>
-    <t>Handel; Instandhaltung und Reparatur von Kraftfahrzeugen und Gebrauchsgütern</t>
-  </si>
-  <si>
-    <t>Verkehr und Nachrichtenübermittlung</t>
-  </si>
-  <si>
-    <t>Kredit- und Versicherungsgewerbe; Grundstücks- und Wohnungswesen, Vermietung beweglicher Sachen, Erbringung von wirt.Dienstleistungen, anderweitig nicht genannt</t>
-  </si>
-  <si>
-    <t>Öffentliche Verwaltung, Verteidigung, Sozialversicherung; Erziehung und Unterricht; Gesundheits-, Veterinär- und Sozialwesen</t>
-  </si>
-  <si>
-    <t>Erbringung von sonstigen öffentlichen und persönlichen Dienstleistungen</t>
-  </si>
-  <si>
-    <t>1) Die Angabe des Wirtschaftszweiges erfolgte ab Erhebungsjahr 2009 nach der Klassifikation der Wirtschaftszweige, Ausgabe 2008 (WZ 2008). Im Jahr 2005 wurde hingegen die zu diesem Zeitpunkt gültige Klassifikation der Wirtschaftszweige, Ausgabe 2003 (WZ 2003), zugrunde gelegt. Aufgrund von größeren Verschiebungen bzw. Änderungen in den fachlichen Zuordnungen sind die dargestellten Werte des Erhebungsjahres 2005 und ab den Jahren 2009 nur sehr eingeschränkt vergleichbar.</t>
-  </si>
-  <si>
     <t xml:space="preserve">2) Hochrechnung anhand der Bevölkerungsfortschreibung auf Basis des Zensus 2011. Die Hochrechnung für die Jahre vor 2011 sowie für bislang veröffentlichte Ergebnisse des Mikrozensus 2011-2013 basiert auf den fortgeschriebenen Ergebnissen der Volkszählung 1987. In 2016 erfolgte die Umstellung auf eine neue Mikrozensus-Stichprobe. Ab 2017 wird nur noch die Bevölkerung in Privathaushalten (ohne Gemeinschaftsunterkünfte) ausgewiesen. Dadurch ergibt sich jeweils eine eingeschränkte Vergleichbarkeit mit den Vorjahren. </t>
   </si>
   <si>
@@ -170,6 +146,9 @@
   </si>
   <si>
     <t>4) Die Ergebnisse des Mikrozensus 2020 sind unter anderem aufgrund methodischer Effekte im Rahmen einer Neugestaltung der Erhebung sowie insbesondere aufgrund der Folgen der Corona-Pandemie in Ihrer Datenqualität eingeschränkt. Auf die Verwendung dieser Ergebnisse wird daher verzichtet. Weitere Informationen zur methodischen Neugestaltung des Mikrozensus ab 2020 und zu den Auswirkungen der Neugestaltung und der Corona-Krise auf die Ergebnisse des Jahres 2020 finden Sie auf der Informationsseite des Statistischen Bundesamtes</t>
+  </si>
+  <si>
+    <t>1) Die Angabe des Wirtschaftszweiges erfolgte ab Erhebungsjahr 2009 nach der Klassifikation der Wirtschaftszweige, Ausgabe 2008 (WZ 2008). Im Jahr 2005 wurde hingegen die zu diesem Zeitpunkt gültige Klassifikation der Wirtschaftszweige, Ausgabe 2003 (WZ 2003), zugrunde gelegt. Aufgrund von größeren Verschiebungen bzw. Änderungen in den fachlichen Zuordnungen sind die dargestellten Werte des Erhebungsjahres 2006 und ab den Jahren 2009 nur sehr eingeschränkt vergleichbar.</t>
   </si>
 </sst>
 </file>
@@ -870,7 +849,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C09ED6D-CD79-470E-91AE-28D4A28E611D}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="B1:F143"/>
+  <dimension ref="B1:F132"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B6" sqref="B6:B9"/>
@@ -2828,283 +2807,96 @@
         <v>553.26731000000007</v>
       </c>
     </row>
-    <row r="121" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B121" s="7" t="s">
+    <row r="121" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B121" s="26"/>
+      <c r="D121" s="14"/>
+      <c r="E121" s="14"/>
+    </row>
+    <row r="122" spans="2:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B122" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="C122" s="42"/>
+      <c r="D122" s="42"/>
+      <c r="E122" s="42"/>
+      <c r="F122" s="42"/>
+    </row>
+    <row r="123" spans="2:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B123" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C121" s="8">
-        <v>2005</v>
-      </c>
-      <c r="D121" s="9">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="E121" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="F121" s="9">
-        <v>11.2</v>
-      </c>
-    </row>
-    <row r="122" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B122" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C122" s="8">
-        <v>2005</v>
-      </c>
-      <c r="D122" s="9">
-        <v>91.5</v>
-      </c>
-      <c r="E122" s="9">
-        <v>34</v>
-      </c>
-      <c r="F122" s="9">
-        <v>125.5</v>
-      </c>
-    </row>
-    <row r="123" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B123" s="7" t="s">
+      <c r="C123" s="27"/>
+      <c r="D123" s="27"/>
+      <c r="E123" s="27"/>
+      <c r="F123" s="28"/>
+    </row>
+    <row r="124" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B124" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="C123" s="8">
-        <v>2005</v>
-      </c>
-      <c r="D123" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E123" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="F123" s="13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="124" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B124" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C124" s="8">
-        <v>2005</v>
-      </c>
-      <c r="D124" s="9">
-        <v>28.3</v>
-      </c>
-      <c r="E124" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="F124" s="9">
-        <v>30.2</v>
-      </c>
-    </row>
-    <row r="125" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B125" s="7" t="s">
+      <c r="C124" s="27"/>
+      <c r="D124" s="27"/>
+      <c r="E124" s="27"/>
+      <c r="F124" s="28"/>
+    </row>
+    <row r="125" spans="2:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B125" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C125" s="27"/>
+      <c r="D125" s="27"/>
+      <c r="E125" s="27"/>
+      <c r="F125" s="27"/>
+    </row>
+    <row r="126" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B126" s="15"/>
+      <c r="D126" s="14"/>
+      <c r="E126" s="14"/>
+    </row>
+    <row r="127" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B127" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C125" s="8">
-        <v>2005</v>
-      </c>
-      <c r="D125" s="9">
-        <v>35.1</v>
-      </c>
-      <c r="E125" s="9">
-        <v>34</v>
-      </c>
-      <c r="F125" s="9">
-        <v>69.099999999999994</v>
-      </c>
-    </row>
-    <row r="126" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B126" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C126" s="8">
-        <v>2005</v>
-      </c>
-      <c r="D126" s="9">
-        <v>23.9</v>
-      </c>
-      <c r="E126" s="9">
-        <v>19.600000000000001</v>
-      </c>
-      <c r="F126" s="9">
-        <v>43.5</v>
-      </c>
-    </row>
-    <row r="127" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B127" s="7" t="s">
+      <c r="C127" s="16"/>
+    </row>
+    <row r="128" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" spans="2:3" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B129" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C127" s="8">
-        <v>2005</v>
-      </c>
-      <c r="D127" s="9">
-        <v>16.5</v>
-      </c>
-      <c r="E127" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="F127" s="9">
-        <v>20.7</v>
-      </c>
-    </row>
-    <row r="128" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B128" s="7" t="s">
+      <c r="C129" s="16"/>
+    </row>
+    <row r="130" spans="2:3" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B130" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C128" s="8">
-        <v>2005</v>
-      </c>
-      <c r="D128" s="9">
-        <v>18.3</v>
-      </c>
-      <c r="E128" s="9">
-        <v>19.600000000000001</v>
-      </c>
-      <c r="F128" s="9">
-        <v>37.9</v>
-      </c>
-    </row>
-    <row r="129" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B129" s="7" t="s">
+      <c r="C130" s="16"/>
+    </row>
+    <row r="131" spans="2:3" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B131" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="C129" s="8">
-        <v>2005</v>
-      </c>
-      <c r="D129" s="9">
-        <v>26.6</v>
-      </c>
-      <c r="E129" s="9">
-        <v>52.5</v>
-      </c>
-      <c r="F129" s="9">
-        <v>79.2</v>
-      </c>
-    </row>
-    <row r="130" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B130" s="7" t="s">
+      <c r="C131" s="16"/>
+    </row>
+    <row r="132" spans="2:3" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B132" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C130" s="8">
-        <v>2005</v>
-      </c>
-      <c r="D130" s="9">
-        <v>13.4</v>
-      </c>
-      <c r="E130" s="9">
-        <v>18.100000000000001</v>
-      </c>
-      <c r="F130" s="9">
-        <v>31.5</v>
-      </c>
-    </row>
-    <row r="131" spans="2:6" s="23" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B131" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C131" s="25">
-        <v>2005</v>
-      </c>
-      <c r="D131" s="21">
-        <v>264.8</v>
-      </c>
-      <c r="E131" s="21">
-        <v>190.2</v>
-      </c>
-      <c r="F131" s="21">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="132" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B132" s="26"/>
-      <c r="D132" s="14"/>
-      <c r="E132" s="14"/>
-    </row>
-    <row r="133" spans="2:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B133" s="42" t="s">
-        <v>29</v>
-      </c>
-      <c r="C133" s="42"/>
-      <c r="D133" s="42"/>
-      <c r="E133" s="42"/>
-      <c r="F133" s="42"/>
-    </row>
-    <row r="134" spans="2:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B134" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="C134" s="27"/>
-      <c r="D134" s="27"/>
-      <c r="E134" s="27"/>
-      <c r="F134" s="28"/>
-    </row>
-    <row r="135" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B135" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="C135" s="27"/>
-      <c r="D135" s="27"/>
-      <c r="E135" s="27"/>
-      <c r="F135" s="28"/>
-    </row>
-    <row r="136" spans="2:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B136" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="C136" s="27"/>
-      <c r="D136" s="27"/>
-      <c r="E136" s="27"/>
-      <c r="F136" s="27"/>
-    </row>
-    <row r="137" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B137" s="15"/>
-      <c r="D137" s="14"/>
-      <c r="E137" s="14"/>
-    </row>
-    <row r="138" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B138" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C138" s="16"/>
-    </row>
-    <row r="139" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="140" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B140" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="C140" s="16"/>
-    </row>
-    <row r="141" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B141" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C141" s="16"/>
-    </row>
-    <row r="142" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B142" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C142" s="16"/>
-    </row>
-    <row r="143" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B143" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C143" s="16"/>
+      <c r="C132" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="B136:F136"/>
-    <mergeCell ref="B135:F135"/>
+    <mergeCell ref="B125:F125"/>
+    <mergeCell ref="B124:F124"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="C6:C9"/>
     <mergeCell ref="D6:F7"/>
     <mergeCell ref="D9:F9"/>
-    <mergeCell ref="B133:F133"/>
-    <mergeCell ref="B134:F134"/>
+    <mergeCell ref="B122:F122"/>
+    <mergeCell ref="B123:F123"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B143" r:id="rId1" xr:uid="{5619BB1D-7346-4B62-96D2-B02C209D90E5}"/>
+    <hyperlink ref="B132" r:id="rId1" xr:uid="{5619BB1D-7346-4B62-96D2-B02C209D90E5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>